<commit_message>
Changes and bugfixes - currently working for all 6 testcases
</commit_message>
<xml_diff>
--- a/test-cases/Example2.xlsx
+++ b/test-cases/Example2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninam\Documents\FAKS\ABSOLVENT\Discrete Math Modeling\Project\Theoretical Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60E05B1-0292-4958-943D-D5965803A78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663889D4-9DBF-4D90-A498-433B3D6005F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5770" yWindow="990" windowWidth="19200" windowHeight="11260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0EE5D0-2230-4D95-BBE0-BB44B7F7C425}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -504,7 +504,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -518,7 +518,7 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>